<commit_message>
experiment 1 first part finalized.
</commit_message>
<xml_diff>
--- a/lab5/2/nMOS_exp2_unflipped.xlsx
+++ b/lab5/2/nMOS_exp2_unflipped.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="nMOS_exp2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1536,11 +1536,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84189184"/>
-        <c:axId val="762895680"/>
+        <c:axId val="48265984"/>
+        <c:axId val="48265408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84189184"/>
+        <c:axId val="48265984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1550,12 +1550,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="762895680"/>
+        <c:crossAx val="48265408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="762895680"/>
+        <c:axId val="48265408"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1567,7 +1567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84189184"/>
+        <c:crossAx val="48265984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1914,7 +1914,7 @@
   <dimension ref="A1:C151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>